<commit_message>
Botton imprimir  y exportar en excel
</commit_message>
<xml_diff>
--- a/DXApplication4/bin/Debug/output.xlsx
+++ b/DXApplication4/bin/Debug/output.xlsx
@@ -4,9 +4,10 @@
   <workbookPr date1904="0"/>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">Sheet!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">Sheet!$A$1:$D$3</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -14,19 +15,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>Numero</t>
   </si>
   <si>
+    <t>Cliente</t>
+  </si>
+  <si>
     <t>Fecha</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>ClienteId</t>
+    <t>Total Factura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFONSO JOSEE  MENDOZA LOVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">john  doe</t>
   </si>
 </sst>
 </file>
@@ -73,18 +77,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -366,38 +367,96 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="35.43" customWidth="1" style="1"/>
-    <col min="2" max="2" width="35.43" customWidth="1" style="2"/>
-    <col min="3" max="3" width="35.43" customWidth="1" style="3"/>
-    <col min="4" max="4" width="35.43" customWidth="1" style="4"/>
-    <col min="5" max="5" width="35.43" customWidth="1" style="2"/>
-    <col min="6" max="6" width="36" customWidth="1" style="1"/>
+    <col min="1" max="1" width="53.29" customWidth="1" style="1"/>
+    <col min="2" max="2" width="53.29" customWidth="1" style="1"/>
+    <col min="3" max="3" width="53.29" customWidth="1" style="2"/>
+    <col min="4" max="4" width="53.29" customWidth="1" style="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c t="s" r="A1" s="2">
+      <c t="s" r="A1" s="3">
         <v>0</v>
       </c>
-      <c t="s" r="B1" s="2">
+      <c t="s" r="B1" s="3">
         <v>1</v>
       </c>
-      <c t="s" r="C1" s="2">
+      <c t="s" r="C1" s="3">
         <v>2</v>
       </c>
-      <c t="s" r="D1" s="2">
+      <c t="s" r="D1" s="3">
         <v>3</v>
       </c>
-      <c t="s" r="E1" s="2">
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c t="s" r="B2" s="1">
         <v>4</v>
       </c>
-      <c t="s" r="F1" s="2">
+      <c r="C2" s="2">
+        <v>44701.791701388887</v>
+      </c>
+      <c r="D2" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
         <v>4</v>
+      </c>
+      <c t="s" r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44701.828032407408</v>
+      </c>
+      <c r="D3" s="3">
+        <v>12150</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:D3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D3" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$B$1:$B$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c t="s" r="B1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" r="B2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError sqref="B1:B2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>